<commit_message>
Add client modal implemented
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -198,7 +198,7 @@
       <xdr:col>30</xdr:col>
       <xdr:colOff>100853</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>14329</xdr:rowOff>
+      <xdr:rowOff>168088</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -208,7 +208,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="14668500" y="1501586"/>
-          <a:ext cx="3585882" cy="8228243"/>
+          <a:ext cx="3585882" cy="8382002"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -339,12 +339,6 @@
           </a:r>
         </a:p>
         <a:p>
-          <a:endParaRPr lang="en-US" sz="2000" baseline="0">
-            <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-            <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="2000" baseline="0">
               <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
@@ -380,7 +374,22 @@
               <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
               <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>adicionar hora a procedimentos</a:t>
+            <a:t>adicionar hora a procedimentos//</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="2000" baseline="0">
+            <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" baseline="0">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>adicionar nome do cliente ao procedimento</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="2000">
             <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
@@ -644,22 +653,37 @@
               <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
               <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>calendario base com semana do dia</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="2000" baseline="0">
-            <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-            <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="2000" baseline="0">
-              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>calendario com datas de procedimentos marcados</a:t>
+            <a:t>calendario base com semana do dia//</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="2000" baseline="0">
+            <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" baseline="0">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>calendario com datas de procedimentos marcados//</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="2000" baseline="0">
+            <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" baseline="0">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>ver detalhes do procedimento (String e cliente) no click do calendario</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -676,6 +700,42 @@
             </a:rPr>
             <a:t>clicar no calendario e gerar um procedimento naquele dia/hora</a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="2000" baseline="0">
+            <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" baseline="0">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>pagina de adicionar cliente</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="2000" baseline="0">
+            <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" baseline="0">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>adicionar procedimento ao cliente</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="2000" baseline="0">
+            <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:endParaRPr lang="en-US" sz="2000" baseline="0">
@@ -1001,8 +1061,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P56" sqref="P56"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AB55" sqref="AB55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
NewProcedure Modal added + Procedure status onClick
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -68,14 +68,14 @@
     <xdr:from>
       <xdr:col>23</xdr:col>
       <xdr:colOff>493058</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>34176</xdr:rowOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>90206</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>30</xdr:col>
       <xdr:colOff>336737</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>22411</xdr:rowOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>78441</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -84,7 +84,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14410764" y="796176"/>
+          <a:off x="14410764" y="90206"/>
           <a:ext cx="4079502" cy="9132235"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -123,14 +123,14 @@
     <xdr:from>
       <xdr:col>25</xdr:col>
       <xdr:colOff>381280</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>11206</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>67236</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>28</xdr:col>
       <xdr:colOff>448516</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>33618</xdr:rowOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>89648</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -139,7 +139,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15509221" y="963706"/>
+          <a:off x="15509221" y="257736"/>
           <a:ext cx="1882589" cy="403412"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -191,14 +191,14 @@
     <xdr:from>
       <xdr:col>24</xdr:col>
       <xdr:colOff>145676</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>168086</xdr:rowOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>33616</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>30</xdr:col>
       <xdr:colOff>100853</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>168088</xdr:rowOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>33618</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -207,7 +207,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14668500" y="1501586"/>
+          <a:off x="14668500" y="795616"/>
           <a:ext cx="3585882" cy="8382002"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -247,7 +247,7 @@
               <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
               <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>o que eu preciso ?</a:t>
+            <a:t>1 cliente com varios procedimentos //</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -262,21 +262,6 @@
               <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
               <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>1 cliente com varios procedimentos //</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="2000">
-            <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-            <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="2000">
-              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-            </a:rPr>
             <a:t>cada cliente precisa ter uma data</a:t>
           </a:r>
           <a:r>
@@ -326,7 +311,7 @@
               <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
               <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>deletar clientes</a:t>
+            <a:t>deletar clientes (CANCELADO)</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -389,7 +374,7 @@
               <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
               <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>adicionar nome do cliente ao procedimento</a:t>
+            <a:t>adicionar nome do cliente ao procedimento//</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="2000">
             <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
@@ -404,14 +389,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>526676</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>34176</xdr:rowOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>90206</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>370355</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>22411</xdr:rowOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>78441</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -420,7 +405,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2947147" y="796176"/>
+          <a:off x="2947147" y="90206"/>
           <a:ext cx="4079502" cy="9132235"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -459,14 +444,14 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>414898</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>11206</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>67236</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>482134</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>33618</xdr:rowOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>89648</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -475,7 +460,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4045604" y="963706"/>
+          <a:off x="4045604" y="257736"/>
           <a:ext cx="1882589" cy="403412"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -527,14 +512,14 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>179295</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>168086</xdr:rowOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>33616</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>134471</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>14329</xdr:rowOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>70359</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -543,7 +528,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3204883" y="1501586"/>
+          <a:off x="3204883" y="795616"/>
           <a:ext cx="3585882" cy="8228243"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -590,40 +575,40 @@
               <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
               <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t> todos os clientes</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="2000" baseline="0">
-              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>exibir todos os procedimentos</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="2000" baseline="0">
-              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>exibir todos os procedimentos de um cliente</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="2000" baseline="0">
-            <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-            <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="2000" baseline="0">
-              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>ordenar procedimentos por data ou valor ou client_id</a:t>
+            <a:t> todos os clientes//</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" baseline="0">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>exibir todos os procedimentos//</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" baseline="0">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>exibir todos os procedimentos de um cliente//</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="2000" baseline="0">
+            <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" baseline="0">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>ordenar procedimentos por data ou valor ou client_id//</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -683,84 +668,449 @@
               <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
               <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>ver detalhes do procedimento (String e cliente) no click do calendario</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="2000" baseline="0">
-            <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-            <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="2000" baseline="0">
-              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+            <a:t>ver detalhes do procedimento (String e cliente) no click do calendario//</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="2000" baseline="0">
+            <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="2000">
+            <a:effectLst/>
+            <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>ordernar por data ou valor pelo clique</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="2000">
+            <a:effectLst/>
+            <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="2000" baseline="0">
+            <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="2000" baseline="0">
+            <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" baseline="0">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>pagina de adicionar cliente//</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="2000" baseline="0">
+            <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" baseline="0">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>adicionar procedimento ao cliente//</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="2000" baseline="0">
+            <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="2000" baseline="0">
+            <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>347381</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>90206</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>191059</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>107492</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="Retângulo 11"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8819028" y="90206"/>
+          <a:ext cx="4079502" cy="10304286"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>235603</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>67236</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>302839</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>89648</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="CaixaDeTexto 12"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9917485" y="257736"/>
+          <a:ext cx="1882589" cy="403412"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Detalhes</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>605117</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>33615</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>560293</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>156882</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="CaixaDeTexto 13"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9076764" y="795615"/>
+          <a:ext cx="3585882" cy="9457767"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>adicionar</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" baseline="0">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> calendario para escolher data</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="2000" baseline="0">
+            <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" baseline="0">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Na hora de comparar datas para  mostra las no calendario, deixar o ano dinamico. atualmente '/2024'</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="2000" baseline="0">
+            <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" baseline="0">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Colocar um metodo melhor de inserir datas para q seja mais facil do usuario acertar</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="2000" baseline="0">
+            <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" baseline="0">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>calendario com horas dinamicas q mudam com zoom </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="2000" baseline="0">
+            <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" baseline="0">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>calendario com eventos dinamicos que mudam com o tempo do evento </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="2000" baseline="0">
+            <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
               <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
             </a:rPr>
             <a:t>clicar no calendario e gerar um procedimento naquele dia/hora</a:t>
           </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="2000" baseline="0">
-            <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-            <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="2000" baseline="0">
-              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>pagina de adicionar cliente</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="2000" baseline="0">
-            <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-            <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="2000" baseline="0">
-              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>adicionar procedimento ao cliente</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="2000" baseline="0">
-            <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-            <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="2000" baseline="0">
-            <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-            <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="2000" baseline="0">
-              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+          <a:endParaRPr lang="en-US" sz="2000">
+            <a:effectLst/>
+            <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="2000" baseline="0">
+            <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" baseline="0">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>deixar bonito</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="2000" baseline="0">
+            <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
               <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
             </a:rPr>
             <a:t>api de envio de emails </a:t>
           </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="2000" baseline="0">
-              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+          <a:endParaRPr lang="en-US" sz="2000">
+            <a:effectLst/>
+            <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
               <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
             </a:rPr>
             <a:t>api de envio de whats app ? </a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="2000">
+            <a:effectLst/>
+            <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="2000" baseline="0">
             <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
             <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
           </a:endParaRPr>
@@ -1061,8 +1411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AB55" sqref="AB55"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Z53" sqref="Z53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Dinamic calendar with click functionalities added
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -568,6 +568,38 @@
               <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
               <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
             </a:rPr>
+            <a:t>Seaach bar para procedimentos</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" baseline="0">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> e pacientes</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="2000">
+            <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="2000">
+            <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="2000">
+            <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
             <a:t>Exibir</a:t>
           </a:r>
           <a:r>
@@ -695,7 +727,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>ordernar por data ou valor pelo clique</a:t>
+            <a:t>ordernar por data ou valor pelo clique//</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="2000">
             <a:effectLst/>
@@ -945,7 +977,7 @@
               <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
               <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t> calendario para escolher data</a:t>
+            <a:t> calendario para escolher data//</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -975,7 +1007,7 @@
               <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
               <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>Colocar um metodo melhor de inserir datas para q seja mais facil do usuario acertar</a:t>
+            <a:t>Colocar um metodo melhor de inserir datas para q seja mais facil do usuario acertar --&gt; mascara</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1114,6 +1146,383 @@
             <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
             <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
           </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>549085</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>67794</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>536863</xdr:colOff>
+      <xdr:row>140</xdr:row>
+      <xdr:rowOff>53862</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="Retângulo 14"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2973630" y="10735794"/>
+          <a:ext cx="4836869" cy="15988068"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>437308</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>44825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>244579</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>67237</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="CaixaDeTexto 15"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4074126" y="10903325"/>
+          <a:ext cx="2231817" cy="403412"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Detalhes</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>201705</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>11202</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>210173</xdr:colOff>
+      <xdr:row>137</xdr:row>
+      <xdr:rowOff>17317</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="CaixaDeTexto 16"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3232387" y="11441202"/>
+          <a:ext cx="4251422" cy="14674615"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>marcar pacientes no clique do calendario --&gt; com barra de pesquisar um usuario ja existente ou para</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" baseline="0">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> criar um novo usuario//</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="2000" baseline="0">
+            <a:effectLst/>
+            <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" baseline="0">
+              <a:effectLst/>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>adicionar uma aba de detalhes para omitir o valor do procedimento</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="2000" baseline="0">
+            <a:effectLst/>
+            <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" baseline="0">
+              <a:effectLst/>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>trocar a palavra valor por orcamento</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="2000" baseline="0">
+            <a:effectLst/>
+            <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" baseline="0">
+              <a:effectLst/>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>trocar a palavra detalhes por tratamento realizado </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="2000" baseline="0">
+            <a:effectLst/>
+            <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" baseline="0">
+              <a:effectLst/>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>quando adicionar um cliente, abrir automaticamente a aba de adicionar procedimentos para esse cliente//</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="2000" baseline="0">
+            <a:effectLst/>
+            <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" baseline="0">
+              <a:effectLst/>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>na aba finanças (todos procedimentos), mostrar apenas os do mes, podendo escolher qual mes se quer ver </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="2000" baseline="0">
+            <a:effectLst/>
+            <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" i="1" baseline="0">
+              <a:effectLst/>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>quando clicar detalhes de um procedimento que está no calendario, poder ja editar direto de la, sem ter q ir na aba de pacientes para tal</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="2000" i="1" baseline="0">
+            <a:effectLst/>
+            <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" i="1" baseline="0">
+              <a:effectLst/>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Adicionar mini calendario sem precisar clicar na data para abrir a selecao de dia</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="2000" baseline="0">
+            <a:effectLst/>
+            <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" baseline="0">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Adicionar um botão de "não marcar" com cor diferente para o calendario//</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="2000" baseline="0">
+            <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" baseline="0">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>adicionar botao de deletar procedimento no calendario</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="2000" baseline="0">
+            <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" baseline="0">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>atualizar aba de financas com data de fim do procedimento, além do botao editar procedimento com data fim</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="2000" baseline="0">
+            <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" baseline="0">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>rabbit mq  // notion</a:t>
+          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -1411,8 +1820,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Z53" sqref="Z53"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="A49" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="R127" sqref="R127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
All functionalities completed (missing aesthetic changes)
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -1156,13 +1156,13 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>549085</xdr:colOff>
       <xdr:row>56</xdr:row>
-      <xdr:rowOff>67794</xdr:rowOff>
+      <xdr:rowOff>67792</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>536863</xdr:colOff>
-      <xdr:row>140</xdr:row>
-      <xdr:rowOff>53862</xdr:rowOff>
+      <xdr:row>157</xdr:row>
+      <xdr:rowOff>64455</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1171,8 +1171,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2973630" y="10735794"/>
-          <a:ext cx="4836869" cy="15988068"/>
+          <a:off x="2973630" y="10735792"/>
+          <a:ext cx="4836869" cy="19237163"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1279,12 +1279,12 @@
       <xdr:col>5</xdr:col>
       <xdr:colOff>201705</xdr:colOff>
       <xdr:row>60</xdr:row>
-      <xdr:rowOff>11202</xdr:rowOff>
+      <xdr:rowOff>11200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>210173</xdr:colOff>
-      <xdr:row>137</xdr:row>
+      <xdr:row>155</xdr:row>
       <xdr:rowOff>17317</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1294,8 +1294,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3232387" y="11441202"/>
-          <a:ext cx="4251422" cy="14674615"/>
+          <a:off x="3232387" y="11441200"/>
+          <a:ext cx="4251422" cy="18103617"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1346,6 +1346,36 @@
         </a:p>
         <a:p>
           <a:endParaRPr lang="en-US" sz="2000" baseline="0">
+            <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" b="1" baseline="0">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>ALTERAR UPDATE PROCEDURE no frontend para ter tb o endDate//</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="2000" b="1" baseline="0">
+            <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" b="1" baseline="0">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>make calendar update automatically after put request from info//</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="2000" baseline="0">
             <a:effectLst/>
             <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
             <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
@@ -1358,7 +1388,7 @@
               <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
               <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>adicionar uma aba de detalhes para omitir o valor do procedimento</a:t>
+            <a:t>adicionar uma aba de detalhes para omitir o valor do procedimento//</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1375,7 +1405,7 @@
               <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
               <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>trocar a palavra valor por orcamento</a:t>
+            <a:t>trocar a palavra valor por orcamento//</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1392,7 +1422,7 @@
               <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
               <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>trocar a palavra detalhes por tratamento realizado </a:t>
+            <a:t>trocar a palavra detalhes por tratamento realizado//</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1428,6 +1458,19 @@
             </a:rPr>
             <a:t>na aba finanças (todos procedimentos), mostrar apenas os do mes, podendo escolher qual mes se quer ver </a:t>
           </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" b="1" baseline="0">
+              <a:effectLst/>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>(FALTA PODER ESCOLHER O MES -&gt; BACKEND FEITO)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="2000" baseline="0">
+            <a:effectLst/>
+            <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:endParaRPr lang="en-US" sz="2000" baseline="0">
@@ -1443,7 +1486,7 @@
               <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
               <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>quando clicar detalhes de um procedimento que está no calendario, poder ja editar direto de la, sem ter q ir na aba de pacientes para tal</a:t>
+            <a:t>quando clicar detalhes de um procedimento que está no calendario, poder ja editar direto de la, sem ter q ir na aba de pacientes para tal//</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1491,22 +1534,51 @@
               <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
               <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>adicionar botao de deletar procedimento no calendario</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="2000" baseline="0">
-            <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-            <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="2000" baseline="0">
-              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>atualizar aba de financas com data de fim do procedimento, além do botao editar procedimento com data fim</a:t>
+            <a:t>adicionar botao de deletar procedimento no calendario//</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="2000" baseline="0">
+            <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" baseline="0">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>atualizar aba de financas com data de fim do procedimento, além do botao editar procedimento com data fim//</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="2000" baseline="0">
+            <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" baseline="0">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Mudar aba de novo procedimento para separar data, hora inicio e hora fim ao inves de ter q </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" u="sng" baseline="0">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>escrever</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" baseline="0">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> a mesma data 2 vezes</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1820,8 +1892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="A49" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="R127" sqref="R127"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="A57" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="O147" sqref="O147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>